<commit_message>
created ICuttable. Deleted Flavoring. Created Salad. Added resourceBundles. Added Salad instances to ChiefCook. Added maven support
</commit_message>
<xml_diff>
--- a/vegetables.xlsx
+++ b/vegetables.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="104">
   <si>
     <t>ПРОДУКТ</t>
   </si>
@@ -239,15 +239,6 @@
     <t>grains</t>
   </si>
   <si>
-    <t>Color</t>
-  </si>
-  <si>
-    <t>RED</t>
-  </si>
-  <si>
-    <t>ORANGE</t>
-  </si>
-  <si>
     <t>TOMATOES</t>
   </si>
   <si>
@@ -272,29 +263,86 @@
     <t>Classification.SALADS</t>
   </si>
   <si>
-    <t>Color.GREEN</t>
-  </si>
-  <si>
-    <t>Color.WHITE</t>
-  </si>
-  <si>
-    <t>Color.VIOLET</t>
-  </si>
-  <si>
-    <t>Color.RED</t>
-  </si>
-  <si>
     <t>Classification.BEAN_FAMILY</t>
   </si>
   <si>
     <t>Classification.GOURD_FAMILY</t>
+  </si>
+  <si>
+    <t>Горчица столовая</t>
+  </si>
+  <si>
+    <t>Майонез «Провансаль», 67% жирности</t>
+  </si>
+  <si>
+    <t>Орегано, сушеный</t>
+  </si>
+  <si>
+    <t>Перец душистый, молотый</t>
+  </si>
+  <si>
+    <t>Розмарин, сушеный</t>
+  </si>
+  <si>
+    <t>Соевый соус</t>
+  </si>
+  <si>
+    <t>Соль столовая</t>
+  </si>
+  <si>
+    <t>Укроп, сушеный</t>
+  </si>
+  <si>
+    <t>Уксус бальзамический</t>
+  </si>
+  <si>
+    <t>Шалфей, молотый</t>
+  </si>
+  <si>
+    <t>mustard</t>
+  </si>
+  <si>
+    <t>mayonnaise</t>
+  </si>
+  <si>
+    <t>Oregano</t>
+  </si>
+  <si>
+    <t>rosemary</t>
+  </si>
+  <si>
+    <t>Soy_sauce</t>
+  </si>
+  <si>
+    <t>salt</t>
+  </si>
+  <si>
+    <t>Dill</t>
+  </si>
+  <si>
+    <t>Vinegar</t>
+  </si>
+  <si>
+    <t>pepper</t>
+  </si>
+  <si>
+    <t>salvia</t>
+  </si>
+  <si>
+    <t>(Classification.SAUCE,</t>
+  </si>
+  <si>
+    <t>(Classification.HERB,</t>
+  </si>
+  <si>
+    <t>(Classification.SEASONING,</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -325,13 +373,26 @@
       <family val="2"/>
       <charset val="204"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="204"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -361,28 +422,32 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -664,611 +729,777 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L20"/>
+  <dimension ref="A1:K30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I1" sqref="I1:J1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="F21" sqref="F21:F30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="5" max="5" width="25.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="3" width="8.88671875" style="4"/>
+    <col min="4" max="4" width="25.5546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="8.88671875" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="6"/>
-      <c r="G1" s="2" t="s">
+      <c r="B1" s="2"/>
+      <c r="C1" s="3"/>
+      <c r="E1" s="5" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A2" s="1"/>
-      <c r="B2" s="1"/>
-      <c r="C2" s="6"/>
-      <c r="F2" t="s">
-        <v>71</v>
-      </c>
-      <c r="G2" s="2" t="s">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A2" s="2"/>
+      <c r="B2" s="2"/>
+      <c r="C2" s="3"/>
+      <c r="E2" s="5" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A3" s="3" t="s">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A3" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="6" t="s">
         <v>38</v>
       </c>
       <c r="C3" s="7" t="str">
         <f>UPPER(B3)</f>
         <v>AUBERGINE</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="D3" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="E3" s="8">
+        <v>24</v>
+      </c>
+      <c r="F3" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="E3" t="s">
-        <v>74</v>
-      </c>
-      <c r="F3" t="s">
-        <v>72</v>
-      </c>
-      <c r="G3" s="4">
-        <v>24</v>
-      </c>
-      <c r="I3" s="5" t="s">
+      <c r="H3" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="J3" s="5" t="s">
+      <c r="I3" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="K3" s="5" t="str">
-        <f>UPPER(J3)</f>
+      <c r="J3" s="1" t="str">
+        <f>UPPER(I3)</f>
         <v>TUBERS</v>
       </c>
-      <c r="L3" t="s">
+      <c r="K3" s="4" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="4" spans="1:12" ht="19.2" x14ac:dyDescent="0.3">
-      <c r="A4" s="3" t="s">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A4" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="6" t="s">
         <v>20</v>
       </c>
       <c r="C4" s="7" t="str">
         <f t="shared" ref="C4:C7" si="0">UPPER(B4)</f>
         <v>GREEN PEAS</v>
       </c>
-      <c r="D4" s="5" t="s">
+      <c r="D4" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="E4" s="8">
+        <v>72</v>
+      </c>
+      <c r="F4" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="E4" t="s">
-        <v>86</v>
-      </c>
-      <c r="F4" t="s">
-        <v>82</v>
-      </c>
-      <c r="G4" s="4">
-        <v>72</v>
-      </c>
-      <c r="I4" s="5" t="s">
+      <c r="H4" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="J4" s="5" t="s">
+      <c r="I4" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="K4" s="5" t="str">
-        <f t="shared" ref="K4:K8" si="1">UPPER(J4)</f>
+      <c r="J4" s="1" t="str">
+        <f t="shared" ref="J4:J8" si="1">UPPER(I4)</f>
         <v>ROOTS</v>
       </c>
-      <c r="L4" t="s">
+      <c r="K4" s="4" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A5" s="3" t="s">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A5" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="6" t="s">
         <v>21</v>
       </c>
       <c r="C5" s="7" t="str">
         <f t="shared" si="0"/>
         <v>ZUCCHINI</v>
       </c>
-      <c r="D5" s="5" t="s">
+      <c r="D5" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="E5" s="8">
+        <v>27</v>
+      </c>
+      <c r="F5" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="E5" t="s">
-        <v>87</v>
-      </c>
-      <c r="F5" t="s">
-        <v>82</v>
-      </c>
-      <c r="G5" s="4">
-        <v>27</v>
-      </c>
-      <c r="I5" s="5" t="s">
+      <c r="H5" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="J5" s="5" t="s">
+      <c r="I5" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="K5" s="5" t="str">
+      <c r="J5" s="1" t="str">
         <f t="shared" si="1"/>
         <v>CABBAGES</v>
       </c>
-      <c r="L5" t="s">
+      <c r="K5" s="4" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="6" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A6" s="3" t="s">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A6" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="6" t="s">
         <v>22</v>
       </c>
       <c r="C6" s="7" t="str">
         <f t="shared" si="0"/>
         <v>WHITE CABBAGE</v>
       </c>
-      <c r="D6" s="5" t="s">
+      <c r="D6" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="E6" s="8">
+        <v>28</v>
+      </c>
+      <c r="F6" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="E6" t="s">
-        <v>75</v>
-      </c>
-      <c r="F6" t="s">
-        <v>83</v>
-      </c>
-      <c r="G6" s="4">
-        <v>28</v>
-      </c>
-      <c r="I6" s="5" t="s">
+      <c r="H6" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="J6" s="5" t="s">
+      <c r="I6" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="K6" s="5" t="str">
+      <c r="J6" s="1" t="str">
         <f t="shared" si="1"/>
         <v>ONIONS</v>
       </c>
-      <c r="L6" t="s">
+      <c r="K6" s="4" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="7" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A7" s="3" t="s">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A7" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="6" t="s">
         <v>23</v>
       </c>
       <c r="C7" s="7" t="str">
         <f t="shared" si="0"/>
         <v>RED CABBAGE</v>
       </c>
-      <c r="D7" s="5" t="s">
+      <c r="D7" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="E7" s="8">
+        <v>31</v>
+      </c>
+      <c r="F7" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="E7" t="s">
-        <v>75</v>
-      </c>
-      <c r="F7" t="s">
-        <v>84</v>
-      </c>
-      <c r="G7" s="4">
-        <v>31</v>
-      </c>
-      <c r="I7" s="5" t="s">
+      <c r="H7" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="J7" s="5" t="s">
+      <c r="I7" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="K7" s="5" t="str">
+      <c r="J7" s="1" t="str">
         <f t="shared" si="1"/>
         <v>SALADS</v>
       </c>
-      <c r="L7" t="s">
+      <c r="K7" s="4" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A8" s="3" t="s">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A8" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B8" s="6" t="s">
         <v>24</v>
       </c>
       <c r="C8" s="7" t="str">
-        <f>UPPER(B8)</f>
+        <f t="shared" ref="C8:C30" si="2">UPPER(B8)</f>
         <v>POTATOES</v>
       </c>
-      <c r="D8" s="5" t="s">
+      <c r="D8" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="E8" s="8">
+        <v>83</v>
+      </c>
+      <c r="F8" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="E8" t="s">
-        <v>76</v>
-      </c>
-      <c r="F8" t="s">
-        <v>83</v>
-      </c>
-      <c r="G8" s="4">
-        <v>83</v>
-      </c>
-      <c r="I8" s="5" t="s">
+      <c r="H8" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="J8" s="5" t="s">
+      <c r="I8" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="K8" s="5" t="str">
+      <c r="J8" s="1" t="str">
         <f t="shared" si="1"/>
         <v>SPICY</v>
       </c>
-      <c r="L8" t="s">
+      <c r="K8" s="4" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="9" spans="1:12" ht="19.2" x14ac:dyDescent="0.3">
-      <c r="A9" s="3" t="s">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A9" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="B9" s="6" t="s">
         <v>25</v>
       </c>
       <c r="C9" s="7" t="str">
-        <f>UPPER(B9)</f>
+        <f t="shared" si="2"/>
         <v xml:space="preserve">GREEN ONION </v>
       </c>
-      <c r="D9" s="5" t="s">
+      <c r="D9" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="E9" s="8">
+        <v>22</v>
+      </c>
+      <c r="F9" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="E9" t="s">
+      <c r="H9" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="K9" s="4" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A10" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="C10" s="7" t="str">
+        <f t="shared" si="2"/>
+        <v>BULB ONIONS</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="E10" s="8">
+        <v>43</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="H10" s="1"/>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A11" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="C11" s="7" t="str">
+        <f t="shared" si="2"/>
+        <v>RED CARROT</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="E11" s="8">
+        <v>33</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="J11" s="1" t="str">
+        <f>UPPER(I11)</f>
+        <v>TOMATOES</v>
+      </c>
+      <c r="K11" s="4" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A12" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="C12" s="7" t="str">
+        <f t="shared" si="2"/>
+        <v>CUCUMBERS</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="E12" s="8">
+        <v>15</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="I12" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="J12" s="1" t="str">
+        <f>UPPER(I12)</f>
+        <v>GOURD FAMILY</v>
+      </c>
+      <c r="K12" s="4" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A13" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="C13" s="7" t="str">
+        <f t="shared" si="2"/>
+        <v>SWEET RED PEPPER</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="E13" s="8">
+        <v>27</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="I13" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="J13" s="1" t="str">
+        <f>UPPER(I13)</f>
+        <v>BEAN FAMILY</v>
+      </c>
+      <c r="K13" s="4" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A14" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="C14" s="7" t="str">
+        <f t="shared" si="2"/>
+        <v>PARSLEY (GREENS)</v>
+      </c>
+      <c r="D14" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="F9" t="s">
+      <c r="E14" s="8">
+        <v>45</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="H14" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="I14" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="J14" s="1" t="str">
+        <f>UPPER(I14)</f>
+        <v>GRAINS</v>
+      </c>
+      <c r="K14" s="4" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A15" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="C15" s="7" t="str">
+        <f t="shared" si="2"/>
+        <v>RADISH</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="E15" s="8">
+        <v>20</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A16" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B16" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="C16" s="7" t="str">
+        <f t="shared" si="2"/>
+        <v>SALAD</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="E16" s="8">
+        <v>14</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A17" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B17" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="C17" s="7" t="str">
+        <f t="shared" si="2"/>
+        <v>BEET</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="E17" s="8">
+        <v>48</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A18" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B18" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="C18" s="7" t="str">
+        <f t="shared" si="2"/>
+        <v>TOMATOES</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="E18" s="8">
+        <v>19</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A19" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B19" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="C19" s="7" t="str">
+        <f t="shared" si="2"/>
+        <v>GREEN BEANS</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="E19" s="8">
+        <v>32</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A20" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B20" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="C20" s="7" t="str">
+        <f t="shared" si="2"/>
+        <v>GARLIC</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="E20" s="8">
+        <v>106</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A21" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="B21" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="C21" s="7" t="str">
+        <f>UPPER(B21)</f>
+        <v>MUSTARD</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="E21" s="8">
+        <v>143</v>
+      </c>
+      <c r="F21" s="1" t="str">
+        <f>CONCATENATE(C21,D21,E21)</f>
+        <v>MUSTARD(Classification.SAUCE,143</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A22" s="6" t="s">
         <v>82</v>
       </c>
-      <c r="G9" s="4">
-        <v>22</v>
-      </c>
-      <c r="I9" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="L9" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" ht="19.2" x14ac:dyDescent="0.3">
-      <c r="A10" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="C10" s="7" t="str">
-        <f>UPPER(B10)</f>
-        <v>BULB ONIONS</v>
-      </c>
-      <c r="D10" s="5" t="s">
+      <c r="B22" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="C22" s="7" t="str">
+        <f t="shared" si="2"/>
+        <v>MAYONNAISE</v>
+      </c>
+      <c r="D22" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="E22" s="8">
+        <v>629</v>
+      </c>
+      <c r="F22" s="1" t="str">
+        <f>CONCATENATE(C22,D22,E22)</f>
+        <v>MAYONNAISE(Classification.SAUCE,629</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A23" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="B23" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="C23" s="7" t="str">
+        <f t="shared" si="2"/>
+        <v>OREGANO</v>
+      </c>
+      <c r="D23" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="E23" s="8">
+        <v>265</v>
+      </c>
+      <c r="F23" s="1" t="str">
+        <f>CONCATENATE(C23,D23,E23)</f>
+        <v>OREGANO(Classification.HERB,265</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A24" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="B24" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="C24" s="7" t="str">
+        <f t="shared" si="2"/>
+        <v>ROSEMARY</v>
+      </c>
+      <c r="D24" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="E24" s="8">
+        <v>331</v>
+      </c>
+      <c r="F24" s="1" t="str">
+        <f>CONCATENATE(C24,D24,E24)</f>
+        <v>ROSEMARY(Classification.HERB,331</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A25" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="B25" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="C25" s="7" t="str">
+        <f t="shared" si="2"/>
+        <v>SOY_SAUCE</v>
+      </c>
+      <c r="D25" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="E25" s="8">
         <v>53</v>
       </c>
-      <c r="E10" t="s">
-        <v>77</v>
-      </c>
-      <c r="F10" t="s">
-        <v>83</v>
-      </c>
-      <c r="G10" s="4">
-        <v>43</v>
-      </c>
-      <c r="I10" s="5"/>
-    </row>
-    <row r="11" spans="1:12" ht="19.2" x14ac:dyDescent="0.3">
-      <c r="A11" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="C11" s="7" t="str">
-        <f>UPPER(B11)</f>
-        <v>RED CARROT</v>
-      </c>
-      <c r="D11" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="E11" t="s">
-        <v>78</v>
-      </c>
-      <c r="F11" t="s">
-        <v>73</v>
-      </c>
-      <c r="G11" s="4">
-        <v>33</v>
-      </c>
-      <c r="I11" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="J11" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="K11" s="5" t="str">
-        <f>UPPER(J11)</f>
-        <v>TOMATOES</v>
-      </c>
-      <c r="L11" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" ht="19.2" x14ac:dyDescent="0.3">
-      <c r="A12" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="C12" s="7" t="str">
-        <f>UPPER(B12)</f>
-        <v>CUCUMBERS</v>
-      </c>
-      <c r="D12" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="E12" t="s">
+      <c r="F25" s="1" t="str">
+        <f>CONCATENATE(C25,D25,E25)</f>
+        <v>SOY_SAUCE(Classification.SAUCE,53</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A26" s="6" t="s">
         <v>87</v>
       </c>
-      <c r="F12" t="s">
-        <v>82</v>
-      </c>
-      <c r="G12" s="4">
-        <v>15</v>
-      </c>
-      <c r="I12" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="J12" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="K12" s="5" t="str">
-        <f>UPPER(J12)</f>
-        <v>GOURD FAMILY</v>
-      </c>
-      <c r="L12" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A13" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="C13" s="7" t="str">
-        <f>UPPER(B13)</f>
-        <v>SWEET RED PEPPER</v>
-      </c>
-      <c r="D13" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="E13" t="s">
-        <v>79</v>
-      </c>
-      <c r="F13" t="s">
-        <v>85</v>
-      </c>
-      <c r="G13" s="4">
-        <v>27</v>
-      </c>
-      <c r="I13" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="J13" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="K13" s="5" t="str">
-        <f>UPPER(J13)</f>
-        <v>BEAN FAMILY</v>
-      </c>
-      <c r="L13" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" ht="19.2" x14ac:dyDescent="0.3">
-      <c r="A14" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="C14" s="7" t="str">
-        <f>UPPER(B14)</f>
-        <v>PARSLEY (GREENS)</v>
-      </c>
-      <c r="D14" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="E14" t="s">
-        <v>80</v>
-      </c>
-      <c r="F14" t="s">
-        <v>82</v>
-      </c>
-      <c r="G14" s="4">
-        <v>45</v>
-      </c>
-      <c r="I14" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="J14" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="K14" s="5" t="str">
-        <f>UPPER(J14)</f>
-        <v>GRAINS</v>
-      </c>
-      <c r="L14" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A15" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="C15" s="7" t="str">
-        <f>UPPER(B15)</f>
-        <v>RADISH</v>
-      </c>
-      <c r="D15" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="E15" t="s">
-        <v>78</v>
-      </c>
-      <c r="F15" t="s">
-        <v>85</v>
-      </c>
-      <c r="G15" s="4">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A16" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="B16" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="C16" s="7" t="str">
-        <f>UPPER(B16)</f>
-        <v>SALAD</v>
-      </c>
-      <c r="D16" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="E16" t="s">
-        <v>81</v>
-      </c>
-      <c r="F16" t="s">
-        <v>82</v>
-      </c>
-      <c r="G16" s="4">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A17" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="B17" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="C17" s="7" t="str">
-        <f>UPPER(B17)</f>
-        <v>BEET</v>
-      </c>
-      <c r="D17" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="E17" t="s">
-        <v>78</v>
-      </c>
-      <c r="F17" t="s">
+      <c r="B26" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="C26" s="7" t="str">
+        <f t="shared" si="2"/>
+        <v>SALT</v>
+      </c>
+      <c r="D26" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="E26" s="8">
+        <v>0</v>
+      </c>
+      <c r="F26" s="1" t="str">
+        <f>CONCATENATE(C26,D26,E26)</f>
+        <v>SALT(Classification.SEASONING,0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A27" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="B27" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="C27" s="7" t="str">
+        <f t="shared" si="2"/>
+        <v>DILL</v>
+      </c>
+      <c r="D27" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="E27" s="8">
+        <v>253</v>
+      </c>
+      <c r="F27" s="1" t="str">
+        <f>CONCATENATE(C27,D27,E27)</f>
+        <v>DILL(Classification.HERB,253</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A28" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="B28" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="C28" s="7" t="str">
+        <f t="shared" si="2"/>
+        <v>VINEGAR</v>
+      </c>
+      <c r="D28" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="E28" s="8">
+        <v>88</v>
+      </c>
+      <c r="F28" s="1" t="str">
+        <f>CONCATENATE(C28,D28,E28)</f>
+        <v>VINEGAR(Classification.SAUCE,88</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A29" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="B29" s="9" t="s">
+        <v>100</v>
+      </c>
+      <c r="C29" s="7" t="str">
+        <f t="shared" si="2"/>
+        <v>SALVIA</v>
+      </c>
+      <c r="D29" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="E29" s="8">
+        <v>315</v>
+      </c>
+      <c r="F29" s="1" t="str">
+        <f>CONCATENATE(C29,D29,E29)</f>
+        <v>SALVIA(Classification.HERB,315</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A30" s="6" t="s">
         <v>84</v>
       </c>
-      <c r="G17" s="4">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" ht="19.2" x14ac:dyDescent="0.3">
-      <c r="A18" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B18" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="C18" s="7" t="str">
-        <f>UPPER(B18)</f>
-        <v>TOMATOES</v>
-      </c>
-      <c r="D18" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="E18" t="s">
-        <v>79</v>
-      </c>
-      <c r="F18" t="s">
-        <v>85</v>
-      </c>
-      <c r="G18" s="4">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" ht="19.2" x14ac:dyDescent="0.3">
-      <c r="A19" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="B19" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="C19" s="7" t="str">
-        <f>UPPER(B19)</f>
-        <v>GREEN BEANS</v>
-      </c>
-      <c r="D19" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="E19" t="s">
-        <v>86</v>
-      </c>
-      <c r="F19" t="s">
-        <v>82</v>
-      </c>
-      <c r="G19" s="4">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A20" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="B20" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="C20" s="7" t="str">
-        <f>UPPER(B20)</f>
-        <v>GARLIC</v>
-      </c>
-      <c r="D20" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="E20" t="s">
-        <v>77</v>
-      </c>
-      <c r="F20" t="s">
-        <v>83</v>
-      </c>
-      <c r="G20" s="4">
-        <v>106</v>
+      <c r="B30" s="9" t="s">
+        <v>99</v>
+      </c>
+      <c r="C30" s="7" t="str">
+        <f t="shared" si="2"/>
+        <v>PEPPER</v>
+      </c>
+      <c r="D30" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="E30" s="8">
+        <v>263</v>
+      </c>
+      <c r="F30" s="1" t="str">
+        <f>CONCATENATE(C30,D30,E30)</f>
+        <v>PEPPER(Classification.SEASONING,263</v>
       </c>
     </row>
   </sheetData>
   <dataConsolidate>
-    <dataRefs count="1">
+    <dataRefs count="2">
       <dataRef ref="E3:G3" sheet="Лист1"/>
+      <dataRef ref="F21" sheet="Лист1"/>
     </dataRefs>
   </dataConsolidate>
   <mergeCells count="2">
@@ -1276,7 +1507,7 @@
     <mergeCell ref="B1:B2"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="J12" r:id="rId1" tooltip="Gourd" display="https://en.wikipedia.org/wiki/Gourd"/>
+    <hyperlink ref="I12" r:id="rId1" tooltip="Gourd" display="https://en.wikipedia.org/wiki/Gourd"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>

</xml_diff>